<commit_message>
Tonnage splits and moves
</commit_message>
<xml_diff>
--- a/PBR Issue AugSept2019/Queries for splits/Details of data for splits moves.xlsx
+++ b/PBR Issue AugSept2019/Queries for splits/Details of data for splits moves.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\IT Projects\LEMIR SW Phase III\Data Migration\Post go-live\01-20 5 facilities to split\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\solid-waste-migration\PBR Issue AugSept2019\Queries for splits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85CDF007-2733-44B4-AC82-EB5B1C567AEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE2636CC-4F2B-4390-8CC0-E2E8D326317A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-2385" windowWidth="19440" windowHeight="15000" xr2:uid="{6173A7DF-0E9F-4CC1-A2EA-FDE39D01FCC7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6173A7DF-0E9F-4CC1-A2EA-FDE39D01FCC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="137">
   <si>
     <t>Updated</t>
   </si>
@@ -229,6 +229,221 @@
   </si>
   <si>
     <t>Dirk Verhoeff (contact 7062772545) dverhoeff@dwswa.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None yet but possibly McIntosh County C&amp;D </t>
+  </si>
+  <si>
+    <t>From FAC ID</t>
+  </si>
+  <si>
+    <t>From FAC NAME</t>
+  </si>
+  <si>
+    <t>From FIS MFL</t>
+  </si>
+  <si>
+    <t>To FAC ID</t>
+  </si>
+  <si>
+    <t>To FAC Name</t>
+  </si>
+  <si>
+    <t>To FIS MFL</t>
+  </si>
+  <si>
+    <t>From Fac Submittals</t>
+  </si>
+  <si>
+    <t>From MFL ID</t>
+  </si>
+  <si>
+    <t>From FIS NAME</t>
+  </si>
+  <si>
+    <t>From FIS subsystems</t>
+  </si>
+  <si>
+    <t>To MFL ID</t>
+  </si>
+  <si>
+    <t>To FIS NAME</t>
+  </si>
+  <si>
+    <t>Updated 2/25/20</t>
+  </si>
+  <si>
+    <t>To FIS subsystems</t>
+  </si>
+  <si>
+    <t>From FAC Name</t>
+  </si>
+  <si>
+    <t>Cherokee County/USA Waste Pine Bluff Landfill</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>028-039D(SL)</t>
+  </si>
+  <si>
+    <t>Pine Bluff Landfill</t>
+  </si>
+  <si>
+    <t>PINE BLUFF LANDFILL</t>
+  </si>
+  <si>
+    <t>LEMIR 2413, GAPDES 02871, IAIP 05700040</t>
+  </si>
+  <si>
+    <t>407281-2148, 415047-2148, 426564-2149, 428888-2148, 440086-2150, 459103-2148</t>
+  </si>
+  <si>
+    <t>LEMIR Application Types:</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>City of LaGrange Landfill</t>
+  </si>
+  <si>
+    <t>141-013D(SL)</t>
+  </si>
+  <si>
+    <t>047-014D(SL)</t>
+  </si>
+  <si>
+    <t>076-020D(MSWL)</t>
+  </si>
+  <si>
+    <t>137-007D(SL)(3)</t>
+  </si>
+  <si>
+    <t>DOUGHERTY COUNTY LANDFILL</t>
+  </si>
+  <si>
+    <t>Dougherty County Landfill</t>
+  </si>
+  <si>
+    <t>HOUSTON COUNTY LANDFILL</t>
+  </si>
+  <si>
+    <t>Houston County Landfill</t>
+  </si>
+  <si>
+    <t>TIFTON TIFT COUNTY LANDFILL</t>
+  </si>
+  <si>
+    <t>Tifton/Tift County Landfill</t>
+  </si>
+  <si>
+    <t>From EI's</t>
+  </si>
+  <si>
+    <t>UST, MSWL (bad)</t>
+  </si>
+  <si>
+    <t>To EI's</t>
+  </si>
+  <si>
+    <t>Scrap Tire, MSWL (good), SW-TT, GW, MM</t>
+  </si>
+  <si>
+    <t>Scrap Tire (inactive), SW Pgm (bad)</t>
+  </si>
+  <si>
+    <t>Scrap Tire, MSWL (good), GW, MM</t>
+  </si>
+  <si>
+    <t>Scrap Tire Sorter</t>
+  </si>
+  <si>
+    <t>Scrap Tire, MSWL, GW, MM</t>
+  </si>
+  <si>
+    <t>408743 -2148, 411420-2148, 425746-2148, 452587-2148, 465705-2147, 435176-2150, 467315-2150</t>
+  </si>
+  <si>
+    <t>CITY OF LAGRANGE LANDFILL</t>
+  </si>
+  <si>
+    <t>LEMIR 6891, LEMIR 9197, GAPDES 01559, IAIP 28500081</t>
+  </si>
+  <si>
+    <t>DOUGHERTY COUNTY FLEMING/GAISSERT RD MSW LANDFILL</t>
+  </si>
+  <si>
+    <t>411419-2148, 414522-2148, 426653-2148, 463234-2148, 428037-2149, 445432-2150, 458582-2150, 451432-2147, 466187-2147, 466192-2145</t>
+  </si>
+  <si>
+    <t>2147 - SW10 - Groundwater Document Submittal Form</t>
+  </si>
+  <si>
+    <t>2148 - SW09 - Solid Waste Disposal and Recycling Report</t>
+  </si>
+  <si>
+    <t>2149 - SW08 - Remaining Capacity Report</t>
+  </si>
+  <si>
+    <t>2150 - SW11 - Periodic Methane Monitoring Report</t>
+  </si>
+  <si>
+    <t>2145 - SW02 - Request for Minor Modication to Solid Waste Handling Permit</t>
+  </si>
+  <si>
+    <t>2141 - SW06 - Financial Assurance</t>
+  </si>
+  <si>
+    <t>409364-2148, 411207-2148, 427142-2148, 452428-2148, 411894-2149, 441024-2145, 449125-2150, 456996-2150, 458034-2147</t>
+  </si>
+  <si>
+    <t>Tina Yearta</t>
+  </si>
+  <si>
+    <t>Scott Addison, then Christopher Smith (since 1/20)</t>
+  </si>
+  <si>
+    <t>NONE SHOWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special case here, is only one GEOS facility for Pine Bluff, it has no FIS MFL ID, and it looks like submissions are being directed to wrong LEMIR facility (2461). Needs PTWS issue. Also note Pine Bluff is big Waste Mgmt submitter/fee payer
+RO's: John Workman, Gene Barnes, Thomas Lewis, </t>
+  </si>
+  <si>
+    <t>Robbie Dunbar</t>
+  </si>
+  <si>
+    <t>TIFTON/TIFT COUNTY LANDFILL</t>
+  </si>
+  <si>
+    <t>409739-2148, 409763-2148, 409851-2148, 411394-2148, 428716-2148, 458534-2148, 409855-2149, 467750-2147</t>
+  </si>
+  <si>
+    <t>Ricky Hobby</t>
+  </si>
+  <si>
+    <t>LEMIR 3613, LEMIR 140837, GAPDES 03634, IAIP 09500095</t>
+  </si>
+  <si>
+    <t>LEMIR 5491, LEMIR 161129, GAPDES 01844</t>
+  </si>
+  <si>
+    <t>LEMIR 6818, LEMIR 163203, GAPDES 04449, GAPDES 000012983</t>
+  </si>
+  <si>
+    <t>Proposed Actions</t>
+  </si>
+  <si>
+    <t>Moves</t>
+  </si>
+  <si>
+    <t>Brenda Hughes
+Kevin Walter (after 8/1/19)</t>
+  </si>
+  <si>
+    <t>2461 or</t>
   </si>
 </sst>
 </file>
@@ -252,15 +467,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -268,14 +501,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,448 +855,972 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1661893A-87E5-48D3-BE06-EF9C13A465BB}">
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="65.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="61.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" customWidth="1"/>
+    <col min="8" max="8" width="49.42578125" style="3" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" customWidth="1"/>
     <col min="13" max="13" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.5703125" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.28515625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="52.5703125" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" style="3" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>43878</v>
+        <v>43887</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="L4" t="s">
+        <v>79</v>
+      </c>
       <c r="O4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="Q6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="R6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="S6" s="5"/>
+      <c r="T6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="U6" s="5"/>
+      <c r="V6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="W6" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>20296</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C6">
+      <c r="C7" s="6">
         <v>7791</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E6">
+      <c r="E7" s="6">
         <v>268508</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G6">
+      <c r="G7" s="6">
         <v>32636</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I6">
+      <c r="I7" s="6">
         <v>7791</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L6">
+      <c r="L7" s="6">
         <v>34727</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O6">
+      <c r="O7" s="6">
         <v>5436</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q6">
+      <c r="Q7" s="6">
         <v>380496</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S7" s="7"/>
+      <c r="T7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T6">
+      <c r="U7" s="7"/>
+      <c r="V7" s="6">
         <v>7791</v>
       </c>
-      <c r="U6">
+      <c r="W7" s="6">
         <v>32636</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>257000</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="6">
         <v>8170</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E7">
+      <c r="E8" s="6">
         <v>268523</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G7">
+      <c r="G8" s="6">
         <v>34799</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I7">
+      <c r="I8" s="6">
         <v>8170</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L7">
+      <c r="L8" s="6">
         <v>34799</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="O7">
+      <c r="O8" s="6">
         <v>6793</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Q7">
+      <c r="Q8" s="6">
         <v>380560</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S8" s="7"/>
+      <c r="T8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="T7">
+      <c r="U8" s="7"/>
+      <c r="V8" s="6">
         <v>8170</v>
       </c>
-      <c r="U7">
+      <c r="W8" s="6">
         <v>34799</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>257049</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C8">
+      <c r="C9" s="6">
         <v>32386</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E8">
+      <c r="E9" s="6">
         <v>267349</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G8">
+      <c r="G9" s="6">
         <v>34728</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I8">
+      <c r="I9" s="6">
         <v>32386</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="L8">
+      <c r="L9" s="6">
         <v>34728</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="O8">
+      <c r="O9" s="6">
         <v>153082</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q8">
+      <c r="Q9" s="6">
         <v>380498</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S9" s="7"/>
+      <c r="T9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="T8">
+      <c r="U9" s="7"/>
+      <c r="V9" s="6">
         <v>32386</v>
       </c>
-      <c r="U8">
+      <c r="W9" s="6">
         <v>34728</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>256680</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C9">
+      <c r="C10" s="6">
         <v>32532</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E9">
+      <c r="E10" s="6">
         <v>268527</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G9">
+      <c r="G10" s="6">
         <v>34726</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I9">
+      <c r="I10" s="6">
         <v>32532</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="L9">
+      <c r="L10" s="6">
         <v>34726</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="O9">
+      <c r="O10" s="6">
         <v>160596</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q9">
+      <c r="Q10" s="6">
         <v>380499</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S10" s="7"/>
+      <c r="T10" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="T9">
+      <c r="U10" s="7"/>
+      <c r="V10" s="6">
         <v>32532</v>
       </c>
-      <c r="U9">
+      <c r="W10" s="6">
         <v>34726</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G10">
+    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>15586</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="6">
+        <v>17122</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="6">
+        <v>268628</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="6">
         <v>34798</v>
       </c>
-      <c r="I10">
+      <c r="H11" s="7"/>
+      <c r="I11" s="6">
         <v>17122</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="L10">
+      <c r="L11" s="6">
         <v>34798</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N11" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O10">
+      <c r="O11" s="6">
         <v>346047</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="Q10">
+      <c r="Q11" s="6">
         <v>380561</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S11" s="7"/>
+      <c r="T11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="T10">
+      <c r="U11" s="7"/>
+      <c r="V11" s="6">
         <v>17122</v>
       </c>
-      <c r="U10">
+      <c r="W11" s="6">
         <v>34798</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="D13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>267</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" s="6">
+        <v>267</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6">
+        <v>506</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="6">
+        <v>506</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="O15" s="6">
+        <v>2461</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>2413</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="T15" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="V15" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="W15" s="8">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>1368</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2781</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" s="6">
+        <v>2781</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="O16" s="6">
+        <v>9197</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>6891</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="T16" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="V16" s="9">
+        <v>2781</v>
+      </c>
+      <c r="W16" s="9">
+        <v>2781</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>546</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1120</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="6">
+        <v>1120</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="O17" s="6">
+        <v>140837</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>3613</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="T17" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="V17" s="9">
+        <v>1120</v>
+      </c>
+      <c r="W17" s="9">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>4336</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="6">
+        <v>10359</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I18" s="6">
+        <v>10359</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="O18" s="6">
+        <v>161129</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>5491</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="T18" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="U18" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="V18" s="9">
+        <v>10359</v>
+      </c>
+      <c r="W18" s="9">
+        <v>10359</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>15519</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="6">
+        <v>8176</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I19" s="6">
+        <v>8176</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="O19" s="6">
+        <v>163203</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>6818</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="T19" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="V19" s="9">
+        <v>8176</v>
+      </c>
+      <c r="W19" s="9">
+        <v>8176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>